<commit_message>
adicao de indice de isolamento social
</commit_message>
<xml_diff>
--- a/Artefatos/Dados Trabalho/Dados Transformados/Isolamento Social/indice-isolamento-social.xlsx
+++ b/Artefatos/Dados Trabalho/Dados Transformados/Isolamento Social/indice-isolamento-social.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raptor\Documents\Faculdade\9º Semestre\Sistemas de Apoio a Decisão\trab-siad\Artefatos\Dados Trabalho\Dados Transformados\Isolamento Social\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\trab-siad\Artefatos\Dados Trabalho\Dados Transformados\Isolamento Social\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9451A31-D93E-4DB9-BEDD-238CF37AF396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{08437A86-17E9-4305-AF5C-9C755253590F}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -388,11 +387,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91B779E-6C2E-4116-9943-9E4FFC2D982C}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,58 +409,938 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43996</v>
+        <v>43887</v>
       </c>
       <c r="B2">
-        <v>48.38</v>
+        <v>24.7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43997</v>
+        <v>43888</v>
       </c>
       <c r="B3">
-        <v>39.33</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>43998</v>
+        <v>43889</v>
       </c>
       <c r="B4">
-        <v>39.56</v>
+        <v>26.6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43999</v>
+        <v>43890</v>
       </c>
       <c r="B5">
-        <v>37.75</v>
+        <v>31.4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>44000</v>
+        <v>43891</v>
       </c>
       <c r="B6">
-        <v>39.01</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>44001</v>
+        <v>43892</v>
       </c>
       <c r="B7">
-        <v>35.020000000000003</v>
+        <v>27.7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
+        <v>43893</v>
+      </c>
+      <c r="B8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43894</v>
+      </c>
+      <c r="B9">
+        <v>30.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43895</v>
+      </c>
+      <c r="B10">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43896</v>
+      </c>
+      <c r="B11">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43897</v>
+      </c>
+      <c r="B12">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43898</v>
+      </c>
+      <c r="B13">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43899</v>
+      </c>
+      <c r="B14">
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43900</v>
+      </c>
+      <c r="B15">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43901</v>
+      </c>
+      <c r="B16">
+        <v>28.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43902</v>
+      </c>
+      <c r="B17">
+        <v>30.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43903</v>
+      </c>
+      <c r="B18">
+        <v>30.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43904</v>
+      </c>
+      <c r="B19">
+        <v>35.700000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43905</v>
+      </c>
+      <c r="B20">
+        <v>42.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43906</v>
+      </c>
+      <c r="B21">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43907</v>
+      </c>
+      <c r="B22">
+        <v>32.799999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43908</v>
+      </c>
+      <c r="B23">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43909</v>
+      </c>
+      <c r="B24">
+        <v>39.299999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43910</v>
+      </c>
+      <c r="B25">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43911</v>
+      </c>
+      <c r="B26">
+        <v>52.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B27">
+        <v>62.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B28">
+        <v>52.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B29">
+        <v>53.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B30">
+        <v>53.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43916</v>
+      </c>
+      <c r="B31">
+        <v>53.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B32">
+        <v>51.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>43918</v>
+      </c>
+      <c r="B33">
+        <v>53.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B34">
+        <v>59.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B35">
+        <v>49.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>43921</v>
+      </c>
+      <c r="B36">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B37">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B38">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B39">
+        <v>47.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>43925</v>
+      </c>
+      <c r="B40">
+        <v>50.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>43926</v>
+      </c>
+      <c r="B41">
+        <v>56.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B42">
+        <v>47.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B43">
+        <v>45.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43929</v>
+      </c>
+      <c r="B44">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B45">
+        <v>44.3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43931</v>
+      </c>
+      <c r="B46">
+        <v>54.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43932</v>
+      </c>
+      <c r="B47">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>43933</v>
+      </c>
+      <c r="B48">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>43934</v>
+      </c>
+      <c r="B49">
+        <v>46.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>43935</v>
+      </c>
+      <c r="B50">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>43936</v>
+      </c>
+      <c r="B51">
+        <v>45.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B52">
+        <v>42.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>43938</v>
+      </c>
+      <c r="B53">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>43939</v>
+      </c>
+      <c r="B54">
+        <v>46.6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>43940</v>
+      </c>
+      <c r="B55">
+        <v>54.6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43941</v>
+      </c>
+      <c r="B56">
+        <v>45.4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>43942</v>
+      </c>
+      <c r="B57">
+        <v>52.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>43943</v>
+      </c>
+      <c r="B58">
+        <v>43.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>43944</v>
+      </c>
+      <c r="B59">
+        <v>44.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>43945</v>
+      </c>
+      <c r="B60">
+        <v>42.3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>43946</v>
+      </c>
+      <c r="B61">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>43947</v>
+      </c>
+      <c r="B62">
+        <v>53.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>43948</v>
+      </c>
+      <c r="B63">
+        <v>44.1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>43949</v>
+      </c>
+      <c r="B64">
+        <v>43.4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>43950</v>
+      </c>
+      <c r="B65">
+        <v>42.3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>43951</v>
+      </c>
+      <c r="B66">
+        <v>41.2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B67">
+        <v>49.7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>43953</v>
+      </c>
+      <c r="B68">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>43954</v>
+      </c>
+      <c r="B69">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>43955</v>
+      </c>
+      <c r="B70">
+        <v>43.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>43956</v>
+      </c>
+      <c r="B71">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>43957</v>
+      </c>
+      <c r="B72">
+        <v>47.4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>43958</v>
+      </c>
+      <c r="B73">
+        <v>43.3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>43959</v>
+      </c>
+      <c r="B74">
+        <v>40.799999999999997</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>43960</v>
+      </c>
+      <c r="B75">
+        <v>43.1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B76">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>43962</v>
+      </c>
+      <c r="B77">
+        <v>43.3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>43963</v>
+      </c>
+      <c r="B78">
+        <v>43.7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>43964</v>
+      </c>
+      <c r="B79">
+        <v>43.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>43965</v>
+      </c>
+      <c r="B80">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>43966</v>
+      </c>
+      <c r="B81">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>43967</v>
+      </c>
+      <c r="B82">
+        <v>45.8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>43968</v>
+      </c>
+      <c r="B83">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>43969</v>
+      </c>
+      <c r="B84">
+        <v>42.7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>43970</v>
+      </c>
+      <c r="B85">
+        <v>42.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>43971</v>
+      </c>
+      <c r="B86">
+        <v>41.7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>43972</v>
+      </c>
+      <c r="B87">
+        <v>42.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>43973</v>
+      </c>
+      <c r="B88">
+        <v>41.2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>43974</v>
+      </c>
+      <c r="B89">
+        <v>45.3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>43975</v>
+      </c>
+      <c r="B90">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>43976</v>
+      </c>
+      <c r="B91">
+        <v>43.9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>43977</v>
+      </c>
+      <c r="B92">
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>43978</v>
+      </c>
+      <c r="B93">
+        <v>41.1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>43979</v>
+      </c>
+      <c r="B94">
+        <v>41.2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>43980</v>
+      </c>
+      <c r="B95">
+        <v>39.200000000000003</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>43981</v>
+      </c>
+      <c r="B96">
+        <v>42.6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>43982</v>
+      </c>
+      <c r="B97">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B98">
+        <v>40.700000000000003</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>43984</v>
+      </c>
+      <c r="B99">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>43985</v>
+      </c>
+      <c r="B100">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>43986</v>
+      </c>
+      <c r="B101">
+        <v>39.1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B102">
+        <v>39.200000000000003</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>43988</v>
+      </c>
+      <c r="B103">
+        <v>40.6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>43989</v>
+      </c>
+      <c r="B104">
+        <v>48.7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>43990</v>
+      </c>
+      <c r="B105">
+        <v>38.200000000000003</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>43991</v>
+      </c>
+      <c r="B106">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>43992</v>
+      </c>
+      <c r="B107">
+        <v>39.299999999999997</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>43993</v>
+      </c>
+      <c r="B108">
+        <v>43.7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>43994</v>
+      </c>
+      <c r="B109">
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>43995</v>
+      </c>
+      <c r="B110">
+        <v>40.1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>43996</v>
+      </c>
+      <c r="B111">
+        <v>48.9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>43997</v>
+      </c>
+      <c r="B112">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>43998</v>
+      </c>
+      <c r="B113">
+        <v>39.1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>43999</v>
+      </c>
+      <c r="B114">
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>44000</v>
+      </c>
+      <c r="B115">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>44001</v>
+      </c>
+      <c r="B116">
+        <v>34.700000000000003</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
         <v>44002</v>
       </c>
-      <c r="B8">
-        <v>39.369999999999997</v>
+      <c r="B117">
+        <v>39.1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>44003</v>
+      </c>
+      <c r="B118">
+        <v>47.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>